<commit_message>
feat: add new metabolic task
- Add task #257: Biosynthesis of vitamin C
</commit_message>
<xml_diff>
--- a/data/metabolicTasks/metabolicTasks_Full.xlsx
+++ b/data/metabolicTasks/metabolicTasks_Full.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonrob/Documents/PostDoc/human-GEM/ComplementaryData/metabolicTasks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haowa/Dropbox/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E00C9CB5-ED7C-FF47-9E86-104D2797EE2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{734A112F-2865-F840-9300-0D6BBED601F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14680" tabRatio="719" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="32120" windowHeight="17800" tabRatio="719" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="19" r:id="rId1"/>
@@ -20,19 +20,11 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">TASKS!$B$1:$R$474</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1247" uniqueCount="593">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1251" uniqueCount="595">
   <si>
     <t>column 1: Name, also describes the function.</t>
   </si>
@@ -1811,12 +1803,18 @@
   </si>
   <si>
     <t>H2O[s];PPi[s]</t>
+  </si>
+  <si>
+    <t>Biosynthesis of Vitamin C (ascorbate)</t>
+  </si>
+  <si>
+    <t>ascorbate[c]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -2430,8 +2428,8 @@
     <cellStyle name="Linked Cell" xfId="35" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="36" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="37"/>
-    <cellStyle name="Note 2" xfId="38"/>
+    <cellStyle name="Normal 2" xfId="37" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
+    <cellStyle name="Note 2" xfId="38" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
     <cellStyle name="Output" xfId="39" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Title" xfId="40" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="41" builtinId="25" customBuiltin="1"/>
@@ -2838,7 +2836,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
@@ -2894,12 +2892,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R658"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A462" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F475" sqref="F475"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -10601,15 +10599,30 @@
         <v>260</v>
       </c>
     </row>
-    <row r="475" spans="1:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="B475" s="23"/>
-      <c r="C475" s="1"/>
-      <c r="D475" s="1"/>
-    </row>
-    <row r="476" spans="1:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="B476" s="23"/>
-      <c r="C476" s="1"/>
-      <c r="D476" s="1"/>
+    <row r="475" spans="1:12" s="17" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="B475" s="22">
+        <v>257</v>
+      </c>
+      <c r="C475" s="18" t="s">
+        <v>593</v>
+      </c>
+      <c r="D475" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="E475" s="16" t="s">
+        <v>242</v>
+      </c>
+      <c r="H475" s="16" t="s">
+        <v>594</v>
+      </c>
+      <c r="I475" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="476" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H476" s="17" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="477" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="B477" s="23"/>

</xml_diff>